<commit_message>
Finished fixing chapter 4
</commit_message>
<xml_diff>
--- a/thesis_validation_files/thesis_validation.xlsx
+++ b/thesis_validation_files/thesis_validation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Actors</t>
   </si>
@@ -39,25 +39,19 @@
     <t>Approx days to complete</t>
   </si>
   <si>
-    <t>Sample UE-WiSAR</t>
-  </si>
-  <si>
-    <t>Complete UE-WiSAR</t>
-  </si>
-  <si>
-    <t>UAS integrated into NAS</t>
-  </si>
-  <si>
     <t>*Time to Model</t>
   </si>
   <si>
-    <t>Full UE-WiSAR</t>
-  </si>
-  <si>
-    <t>XML UAS in NAS</t>
-  </si>
-  <si>
     <t>*Lines of Code</t>
+  </si>
+  <si>
+    <t>Sample WiSAR</t>
+  </si>
+  <si>
+    <t>Full WiSAR</t>
+  </si>
+  <si>
+    <t>UAS in NAS</t>
   </si>
 </sst>
 </file>
@@ -173,7 +167,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sample UE-WiSAR</c:v>
+                  <c:v>Sample WiSAR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -218,7 +212,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Full UE-WiSAR</c:v>
+                  <c:v>Full WiSAR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -263,7 +257,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>XML UAS in NAS</c:v>
+                  <c:v>UAS in NAS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -309,11 +303,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="43966464"/>
-        <c:axId val="43968000"/>
+        <c:axId val="103232256"/>
+        <c:axId val="103233792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43966464"/>
+        <c:axId val="103232256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -323,7 +317,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43968000"/>
+        <c:crossAx val="103233792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -331,7 +325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43968000"/>
+        <c:axId val="103233792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +335,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43966464"/>
+        <c:crossAx val="103232256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -688,7 +682,7 @@
   <dimension ref="E13:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +695,7 @@
   <sheetData>
     <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1">
         <f>F18/F18</f>
@@ -718,7 +712,7 @@
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1">
         <f>F16/F16</f>
@@ -778,18 +772,18 @@
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
         <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <f>80+450+250+130+50+25+25</f>
@@ -810,7 +804,7 @@
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F23">
         <v>4400</v>
@@ -830,7 +824,7 @@
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F24">
         <v>1250</v>

</xml_diff>